<commit_message>
Tags og færdig 2010
Tilføjelser af tags øverst i sheetsene
</commit_message>
<xml_diff>
--- a/AGR & IND - Jonathans kladder/Hjælpefiler/Simplified_nrg_bal_2010.xlsx
+++ b/AGR & IND - Jonathans kladder/Hjælpefiler/Simplified_nrg_bal_2010.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="564" windowWidth="15996" windowHeight="10524"/>
+    <workbookView xWindow="420" yWindow="564" windowWidth="15996" windowHeight="10524" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="Structure" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet 1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="84">
   <si>
     <t>Simplified energy balances [NRG_BAL_S__custom_2308048]</t>
   </si>
@@ -220,6 +220,54 @@
   </si>
   <si>
     <t>not applicable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Industry and construction </t>
+  </si>
+  <si>
+    <t>Iron and steel</t>
+  </si>
+  <si>
+    <t>Chemical and petrochemical</t>
+  </si>
+  <si>
+    <t>Non-ferrous metal</t>
+  </si>
+  <si>
+    <t>Non-metallic minerals</t>
+  </si>
+  <si>
+    <t>Transport equipment</t>
+  </si>
+  <si>
+    <t>Machinery</t>
+  </si>
+  <si>
+    <t>Mining and quarrying</t>
+  </si>
+  <si>
+    <t>Food and tobacco</t>
+  </si>
+  <si>
+    <t>Paper, pulp and printing</t>
+  </si>
+  <si>
+    <t>Wood and wood products</t>
+  </si>
+  <si>
+    <t>Textile and leather</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Non-specified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agriculture, forestry and fishing </t>
+  </si>
+  <si>
+    <t>Sum af Reneawbles og non-renewables</t>
   </si>
 </sst>
 </file>
@@ -228,9 +276,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.##########"/>
-    <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -264,8 +312,24 @@
       <color indexed="12"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -297,8 +361,14 @@
         <fgColor rgb="FFF6F6F6"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB7ECFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -321,11 +391,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -376,11 +462,14 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -395,12 +484,29 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 3 10 3" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFB7ECFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -741,7 +847,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:O16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -769,22 +875,22 @@
       <c r="A8" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="21"/>
-      <c r="M8" s="21"/>
-      <c r="N8" s="21"/>
-      <c r="O8" s="21"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="22"/>
+      <c r="J8" s="22"/>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="22"/>
+      <c r="N8" s="22"/>
+      <c r="O8" s="22"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1135,18 +1241,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z30"/>
+  <dimension ref="A1:Z44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="10" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="10" topLeftCell="D11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="G26" sqref="G9:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="29.88671875" customWidth="1"/>
+    <col min="1" max="1" width="29.88671875" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="45.5546875" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
     <col min="5" max="5" width="17.88671875" customWidth="1"/>
@@ -1211,162 +1318,162 @@
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="23" t="s">
+      <c r="D8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="F8" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" s="23" t="s">
+      <c r="F8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="I8" s="23" t="s">
+      <c r="H8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="J8" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" s="23" t="s">
+      <c r="J8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="L8" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="M8" s="23" t="s">
+      <c r="L8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="N8" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="O8" s="23" t="s">
+      <c r="N8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="O8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="P8" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q8" s="23" t="s">
+      <c r="P8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="R8" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="S8" s="23" t="s">
+      <c r="R8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="S8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="T8" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="U8" s="23" t="s">
+      <c r="T8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="U8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="V8" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="W8" s="23" t="s">
+      <c r="V8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="W8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="X8" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y8" s="23" t="s">
+      <c r="X8" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="Z8" s="23" t="s">
+      <c r="Z8" s="24" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="24" t="s">
+      <c r="D9" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="G9" s="24" t="s">
+      <c r="F9" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="24" t="s">
+      <c r="H9" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="K9" s="24" t="s">
+      <c r="J9" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="M9" s="24" t="s">
+      <c r="L9" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="M9" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="N9" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="O9" s="24" t="s">
+      <c r="N9" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="P9" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q9" s="24" t="s">
+      <c r="P9" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q9" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="R9" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="S9" s="24" t="s">
+      <c r="R9" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="S9" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="T9" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="U9" s="24" t="s">
+      <c r="T9" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="U9" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="V9" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="W9" s="24" t="s">
+      <c r="V9" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="W9" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="X9" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y9" s="24" t="s">
+      <c r="X9" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y9" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="Z9" s="24" t="s">
+      <c r="Z9" s="25" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1454,8 +1561,8 @@
       <c r="A11" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>22</v>
+      <c r="B11" s="26" t="s">
+        <v>68</v>
       </c>
       <c r="C11" s="14">
         <v>2372614.094</v>
@@ -1534,8 +1641,8 @@
       <c r="A12" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>23</v>
+      <c r="B12" s="27" t="s">
+        <v>69</v>
       </c>
       <c r="C12" s="15">
         <v>330774.06900000002</v>
@@ -1614,8 +1721,8 @@
       <c r="A13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>24</v>
+      <c r="B13" s="27" t="s">
+        <v>70</v>
       </c>
       <c r="C13" s="14">
         <v>588419.799</v>
@@ -1694,8 +1801,8 @@
       <c r="A14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>25</v>
+      <c r="B14" s="27" t="s">
+        <v>71</v>
       </c>
       <c r="C14" s="15">
         <v>89446.138000000006</v>
@@ -1774,8 +1881,8 @@
       <c r="A15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>26</v>
+      <c r="B15" s="27" t="s">
+        <v>72</v>
       </c>
       <c r="C15" s="14">
         <v>272879.16200000001</v>
@@ -1854,8 +1961,8 @@
       <c r="A16" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>27</v>
+      <c r="B16" s="27" t="s">
+        <v>73</v>
       </c>
       <c r="C16" s="15">
         <v>123559.23299999999</v>
@@ -1934,8 +2041,8 @@
       <c r="A17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>28</v>
+      <c r="B17" s="27" t="s">
+        <v>74</v>
       </c>
       <c r="C17" s="14">
         <v>232432.842</v>
@@ -2014,8 +2121,8 @@
       <c r="A18" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>29</v>
+      <c r="B18" s="28" t="s">
+        <v>75</v>
       </c>
       <c r="C18" s="15">
         <v>18503.191999999999</v>
@@ -2094,8 +2201,8 @@
       <c r="A19" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B19" s="5" t="s">
-        <v>30</v>
+      <c r="B19" s="28" t="s">
+        <v>76</v>
       </c>
       <c r="C19" s="14">
         <v>201710.19500000001</v>
@@ -2174,8 +2281,8 @@
       <c r="A20" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>31</v>
+      <c r="B20" s="28" t="s">
+        <v>77</v>
       </c>
       <c r="C20" s="15">
         <v>262458.24099999998</v>
@@ -2254,8 +2361,8 @@
       <c r="A21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>32</v>
+      <c r="B21" s="27" t="s">
+        <v>78</v>
       </c>
       <c r="C21" s="14">
         <v>75463.909</v>
@@ -2334,79 +2441,79 @@
       <c r="A22" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" s="15">
-        <v>36138.853999999999</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E22" s="19">
-        <v>0</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G22" s="19">
-        <v>0</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="I22" s="19">
-        <v>0</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="K22" s="19">
-        <v>0</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="M22" s="15">
-        <v>21828.853999999999</v>
-      </c>
-      <c r="N22" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="O22" s="19">
-        <v>0</v>
-      </c>
-      <c r="P22" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q22" s="19">
-        <v>0</v>
-      </c>
-      <c r="R22" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="S22" s="19">
-        <v>0</v>
-      </c>
-      <c r="T22" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="U22" s="8" t="s">
+      <c r="B22" s="28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C22" s="14">
+        <v>24704.761999999999</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="14">
+        <v>426.83199999999999</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G22" s="18">
+        <v>0</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I22" s="18">
+        <v>0</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K22" s="18">
+        <v>0</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="M22" s="14">
+        <v>10936.927</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="O22" s="14">
+        <v>1781.8030000000001</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q22" s="18">
+        <v>103</v>
+      </c>
+      <c r="R22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S22" s="18">
+        <v>0</v>
+      </c>
+      <c r="T22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="U22" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="V22" s="8" t="s">
+      <c r="V22" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="W22" s="19">
-        <v>14310</v>
-      </c>
-      <c r="X22" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y22" s="19">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="8" t="s">
+      <c r="W22" s="18">
+        <v>8935.2000000000007</v>
+      </c>
+      <c r="X22" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y22" s="18">
+        <v>2521</v>
+      </c>
+      <c r="Z22" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2414,79 +2521,79 @@
       <c r="A23" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C23" s="14">
-        <v>24704.761999999999</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" s="14">
-        <v>426.83199999999999</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G23" s="18">
-        <v>0</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I23" s="18">
-        <v>0</v>
-      </c>
-      <c r="J23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K23" s="18">
-        <v>0</v>
-      </c>
-      <c r="L23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="M23" s="14">
-        <v>10936.927</v>
-      </c>
-      <c r="N23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="O23" s="14">
-        <v>1781.8030000000001</v>
-      </c>
-      <c r="P23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q23" s="18">
-        <v>103</v>
-      </c>
-      <c r="R23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="S23" s="18">
-        <v>0</v>
-      </c>
-      <c r="T23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="U23" s="7" t="s">
+      <c r="B23" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="15">
+        <v>36138.853999999999</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="19">
+        <v>0</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="19">
+        <v>0</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="I23" s="19">
+        <v>0</v>
+      </c>
+      <c r="J23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="K23" s="19">
+        <v>0</v>
+      </c>
+      <c r="L23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="M23" s="15">
+        <v>21828.853999999999</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="O23" s="19">
+        <v>0</v>
+      </c>
+      <c r="P23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q23" s="19">
+        <v>0</v>
+      </c>
+      <c r="R23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="S23" s="19">
+        <v>0</v>
+      </c>
+      <c r="T23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="U23" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="V23" s="7" t="s">
+      <c r="V23" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="W23" s="18">
-        <v>8935.2000000000007</v>
-      </c>
-      <c r="X23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y23" s="18">
-        <v>2521</v>
-      </c>
-      <c r="Z23" s="7" t="s">
+      <c r="W23" s="19">
+        <v>14310</v>
+      </c>
+      <c r="X23" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y23" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="8" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2494,8 +2601,8 @@
       <c r="A24" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>35</v>
+      <c r="B24" s="27" t="s">
+        <v>81</v>
       </c>
       <c r="C24" s="15">
         <v>116123.69500000001</v>
@@ -2574,79 +2681,82 @@
       <c r="A25" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="14">
+      <c r="B25" s="29"/>
+    </row>
+    <row r="26" spans="1:26" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="14">
         <v>53893.033000000003</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E25" s="18">
-        <v>0</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G25" s="18">
-        <v>0</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="I25" s="18">
-        <v>0</v>
-      </c>
-      <c r="J25" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K25" s="18">
-        <v>0</v>
-      </c>
-      <c r="L25" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="M25" s="14">
+      <c r="D26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E26" s="18">
+        <v>0</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G26" s="18">
+        <v>0</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="I26" s="18">
+        <v>0</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K26" s="18">
+        <v>0</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="M26" s="14">
         <v>13816.061</v>
       </c>
-      <c r="N25" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="O25" s="18">
-        <v>0</v>
-      </c>
-      <c r="P25" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q25" s="14">
+      <c r="N26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="O26" s="18">
+        <v>0</v>
+      </c>
+      <c r="P26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q26" s="14">
         <v>18923.371999999999</v>
       </c>
-      <c r="R25" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="S25" s="18">
-        <v>0</v>
-      </c>
-      <c r="T25" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="U25" s="7" t="s">
+      <c r="R26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="S26" s="18">
+        <v>0</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="U26" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="V25" s="7" t="s">
+      <c r="V26" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="W25" s="18">
+      <c r="W26" s="18">
         <v>21153.599999999999</v>
       </c>
-      <c r="X25" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="Y25" s="18">
-        <v>0</v>
-      </c>
-      <c r="Z25" s="7" t="s">
+      <c r="X26" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Y26" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2662,11 +2772,18 @@
       <c r="B28" s="2" t="s">
         <v>65</v>
       </c>
+      <c r="Q28" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="Q29" s="30">
+        <f>Q11+S11</f>
+        <v>152304.52000000002</v>
+      </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
@@ -2675,15 +2792,101 @@
       <c r="B30" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="Q30" s="30">
+        <f t="shared" ref="Q30:Q43" si="0">Q12+S12</f>
+        <v>134.768</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q31" s="30">
+        <f t="shared" si="0"/>
+        <v>13253.46</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q32" s="30">
+        <f t="shared" si="0"/>
+        <v>329</v>
+      </c>
+    </row>
+    <row r="33" spans="17:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q33" s="30">
+        <f t="shared" si="0"/>
+        <v>40433.835999999996</v>
+      </c>
+    </row>
+    <row r="34" spans="17:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q34" s="30">
+        <f t="shared" si="0"/>
+        <v>340.07600000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="17:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q35" s="30">
+        <f t="shared" si="0"/>
+        <v>1857.46</v>
+      </c>
+    </row>
+    <row r="36" spans="17:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q36" s="30">
+        <f t="shared" si="0"/>
+        <v>638.38400000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="17:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q37" s="30">
+        <f t="shared" si="0"/>
+        <v>2386.8440000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="17:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q38" s="30">
+        <f t="shared" si="0"/>
+        <v>42786</v>
+      </c>
+    </row>
+    <row r="39" spans="17:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q39" s="30">
+        <f t="shared" si="0"/>
+        <v>45952</v>
+      </c>
+    </row>
+    <row r="40" spans="17:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q40" s="30">
+        <f t="shared" si="0"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="17:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q41" s="30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="17:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q42" s="30">
+        <f>Q24+S24</f>
+        <v>4089.692</v>
+      </c>
+    </row>
+    <row r="43" spans="17:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q43" s="30">
+        <f>Q25+S25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="17:17" ht="11.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q44" s="30">
+        <f>Q26+S26</f>
+        <v>18923.371999999999</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="13">
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="C8:Z8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:H9"/>
     <mergeCell ref="I9:J9"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="M9:N9"/>

</xml_diff>